<commit_message>
Used solution from Diarmuid Early. Seemed to work.
</commit_message>
<xml_diff>
--- a/CH-076 Reverse Stepped Tax.xlsx
+++ b/CH-076 Reverse Stepped Tax.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D297715D-8CF2-4680-9B75-1168A7732A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2D05C7-DBC3-4115-A65B-B12626E40DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Question</t>
   </si>
@@ -378,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -452,6 +476,9 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1066,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1741,4 +1768,769 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DC6B74-8320-4033-A242-06DF60A305BB}">
+  <dimension ref="A1:O111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.19921875" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="F1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="33"/>
+      <c r="H1" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="26">
+        <v>0</v>
+      </c>
+      <c r="C3" s="27">
+        <v>18200</v>
+      </c>
+      <c r="D3" s="28">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="24">
+        <v>60630</v>
+      </c>
+      <c r="H3" s="25">
+        <v>199920</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3"/>
+      <c r="O3"/>
+    </row>
+    <row r="4" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <f t="shared" ref="B4:B7" si="0">C3+1</f>
+        <v>18201</v>
+      </c>
+      <c r="C4" s="13">
+        <v>45000</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.19</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="16">
+        <v>1495</v>
+      </c>
+      <c r="H4" s="21">
+        <v>26068</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4"/>
+      <c r="O4"/>
+    </row>
+    <row r="5" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <f t="shared" si="0"/>
+        <v>45001</v>
+      </c>
+      <c r="C5" s="13">
+        <v>120000</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="16">
+        <v>25059</v>
+      </c>
+      <c r="H5" s="20">
+        <v>106439</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5"/>
+      <c r="O5"/>
+    </row>
+    <row r="6" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <f t="shared" si="0"/>
+        <v>120001</v>
+      </c>
+      <c r="C6" s="13">
+        <v>180000</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.37</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="16">
+        <v>1961</v>
+      </c>
+      <c r="H6" s="20">
+        <v>28521</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6"/>
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="14">
+        <f t="shared" si="0"/>
+        <v>180001</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="17">
+        <v>37816</v>
+      </c>
+      <c r="H7" s="22">
+        <v>142566</v>
+      </c>
+      <c r="K7"/>
+      <c r="O7"/>
+    </row>
+    <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="4"/>
+      <c r="D8"/>
+      <c r="E8" s="6"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="4"/>
+      <c r="D9"/>
+      <c r="E9" s="6"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="O9"/>
+    </row>
+    <row r="10" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="4"/>
+      <c r="D10"/>
+      <c r="E10" s="6"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+    </row>
+    <row r="11" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="4"/>
+      <c r="D11"/>
+      <c r="E11" s="6"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+    </row>
+    <row r="12" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="30" t="str" cm="1">
+        <f t="array" ref="D12:F17">_xlfn.VSTACK(F2:H2,_xlfn.HSTACK(F3:G7,B13:B17))</f>
+        <v>Person ID</v>
+      </c>
+      <c r="E12" s="30" t="str">
+        <v>Tax</v>
+      </c>
+      <c r="F12" s="31" t="str">
+        <v>Income</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="34" cm="1">
+        <f t="array" ref="B13">_xlfn.LAMBDA(_xlpm.income,_xlpm.brackLow,_xlpm.rat,
+    _xlfn.LET(
+        _xlpm.brackHigh, _xlfn.VSTACK(_xlfn.DROP(_xlpm.brackLow, 1), _xlpm.income),
+        _xlpm.inBand, IF(_xlpm.income &lt; _xlpm.brackLow, 0, IF(_xlpm.income &gt; _xlpm.brackHigh, _xlpm.brackHigh, _xlpm.income) - _xlpm.brackLow),
+        SUM(_xlpm.inBand * _xlpm.rat)
+    )
+)(H3,$B$3:$B$7,$D$3:$D$7)</f>
+        <v>60630.55</v>
+      </c>
+      <c r="D13" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="E13" s="24">
+        <v>60630</v>
+      </c>
+      <c r="F13" s="25">
+        <v>60630.55</v>
+      </c>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="34" cm="1">
+        <f t="array" ref="B14">_xlfn.LAMBDA(_xlpm.income,_xlpm.brackLow,_xlpm.rat,
+    _xlfn.LET(
+        _xlpm.brackHigh, _xlfn.VSTACK(_xlfn.DROP(_xlpm.brackLow, 1), _xlpm.income),
+        _xlpm.inBand, IF(_xlpm.income &lt; _xlpm.brackLow, 0, IF(_xlpm.income &gt; _xlpm.brackHigh, _xlpm.brackHigh, _xlpm.income) - _xlpm.brackLow),
+        SUM(_xlpm.inBand * _xlpm.rat)
+    )
+)(H4,$B$3:$B$7,$D$3:$D$7)</f>
+        <v>1494.73</v>
+      </c>
+      <c r="D14" s="18" t="str">
+        <v>B</v>
+      </c>
+      <c r="E14" s="16">
+        <v>1495</v>
+      </c>
+      <c r="F14" s="21">
+        <v>1494.73</v>
+      </c>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="34" cm="1">
+        <f t="array" ref="B15">_xlfn.LAMBDA(_xlpm.income,_xlpm.brackLow,_xlpm.rat,
+    _xlfn.LET(
+        _xlpm.brackHigh, _xlfn.VSTACK(_xlfn.DROP(_xlpm.brackLow, 1), _xlpm.income),
+        _xlpm.inBand, IF(_xlpm.income &lt; _xlpm.brackLow, 0, IF(_xlpm.income &gt; _xlpm.brackHigh, _xlpm.brackHigh, _xlpm.income) - _xlpm.brackLow),
+        SUM(_xlpm.inBand * _xlpm.rat)
+    )
+)(H5,$B$3:$B$7,$D$3:$D$7)</f>
+        <v>25059.350000000002</v>
+      </c>
+      <c r="D15" s="18" t="str">
+        <v>C</v>
+      </c>
+      <c r="E15" s="16">
+        <v>25059</v>
+      </c>
+      <c r="F15" s="20">
+        <v>25059.350000000002</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="34" cm="1">
+        <f t="array" ref="B16">_xlfn.LAMBDA(_xlpm.income,_xlpm.brackLow,_xlpm.rat,
+    _xlfn.LET(
+        _xlpm.brackHigh, _xlfn.VSTACK(_xlfn.DROP(_xlpm.brackLow, 1), _xlpm.income),
+        _xlpm.inBand, IF(_xlpm.income &lt; _xlpm.brackLow, 0, IF(_xlpm.income &gt; _xlpm.brackHigh, _xlpm.brackHigh, _xlpm.income) - _xlpm.brackLow),
+        SUM(_xlpm.inBand * _xlpm.rat)
+    )
+)(H6,$B$3:$B$7,$D$3:$D$7)</f>
+        <v>1960.8</v>
+      </c>
+      <c r="D16" s="18" t="str">
+        <v>D</v>
+      </c>
+      <c r="E16" s="16">
+        <v>1961</v>
+      </c>
+      <c r="F16" s="20">
+        <v>1960.8</v>
+      </c>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="34" cm="1">
+        <f t="array" ref="B17">_xlfn.LAMBDA(_xlpm.income,_xlpm.brackLow,_xlpm.rat,
+    _xlfn.LET(
+        _xlpm.brackHigh, _xlfn.VSTACK(_xlfn.DROP(_xlpm.brackLow, 1), _xlpm.income),
+        _xlpm.inBand, IF(_xlpm.income &lt; _xlpm.brackLow, 0, IF(_xlpm.income &gt; _xlpm.brackHigh, _xlpm.brackHigh, _xlpm.income) - _xlpm.brackLow),
+        SUM(_xlpm.inBand * _xlpm.rat)
+    )
+)(H7,$B$3:$B$7,$D$3:$D$7)</f>
+        <v>37816.050000000003</v>
+      </c>
+      <c r="D17" s="19" t="str">
+        <v>E</v>
+      </c>
+      <c r="E17" s="17">
+        <v>37816</v>
+      </c>
+      <c r="F17" s="22">
+        <v>37816.050000000003</v>
+      </c>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="9"/>
+      <c r="F18"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="9"/>
+      <c r="E19" s="7"/>
+      <c r="F19"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="9"/>
+      <c r="E20" s="1"/>
+      <c r="F20"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="9"/>
+      <c r="E21" s="1"/>
+      <c r="F21"/>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="9"/>
+      <c r="E22" s="1"/>
+      <c r="F22"/>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="9"/>
+      <c r="E23" s="1"/>
+      <c r="F23"/>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="E24" s="1"/>
+      <c r="F24"/>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+      <c r="E25" s="1"/>
+      <c r="F25"/>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="F26"/>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="F27"/>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
+      <c r="F28"/>
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="F29"/>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+      <c r="F30"/>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="F31"/>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
+      <c r="F32"/>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="F33"/>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="F34"/>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="F35"/>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="F36"/>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="F37"/>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="9"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="9"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="9"/>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="9"/>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="9"/>
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="9"/>
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="9"/>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="9"/>
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="9"/>
+      <c r="F52" s="9"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="9"/>
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="9"/>
+      <c r="F54" s="9"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="9"/>
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="9"/>
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="9"/>
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="9"/>
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="9"/>
+      <c r="F59" s="9"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="9"/>
+      <c r="F60" s="9"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="9"/>
+      <c r="F61" s="9"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="9"/>
+      <c r="F62" s="9"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="9"/>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="9"/>
+      <c r="F64" s="9"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="9"/>
+      <c r="F65" s="9"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="9"/>
+      <c r="F66" s="9"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="9"/>
+      <c r="F67" s="9"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="9"/>
+      <c r="F68" s="9"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="9"/>
+      <c r="F69" s="9"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="9"/>
+      <c r="F70" s="9"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="9"/>
+      <c r="F71" s="9"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="9"/>
+      <c r="F72" s="9"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="9"/>
+      <c r="F73" s="9"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="9"/>
+      <c r="F74" s="9"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="9"/>
+      <c r="F75" s="9"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="9"/>
+      <c r="F76" s="9"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="9"/>
+      <c r="F77" s="9"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="9"/>
+      <c r="F78" s="9"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="9"/>
+      <c r="F79" s="9"/>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="9"/>
+      <c r="F80" s="9"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="9"/>
+      <c r="F81" s="9"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="9"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F83" s="9"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="9"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="9"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="9"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F87" s="9"/>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F88" s="9"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="9"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="9"/>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="9"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="9"/>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F93" s="9"/>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="9"/>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F95" s="9"/>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F96" s="9"/>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="9"/>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="9"/>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="9"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="9"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F101" s="9"/>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F102" s="9"/>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F103" s="9"/>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F104" s="9"/>
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F105" s="9"/>
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F106" s="9"/>
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F107" s="9"/>
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F108" s="9"/>
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F109" s="9"/>
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F110" s="9"/>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F111" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Looked at building a model
</commit_message>
<xml_diff>
--- a/CH-076 Reverse Stepped Tax.xlsx
+++ b/CH-076 Reverse Stepped Tax.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2D05C7-DBC3-4115-A65B-B12626E40DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892CB068-4B71-4060-A1F2-B1362BA1A7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="ModelApproach" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ModelApproach!$B$2:$D$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$7</definedName>
+    <definedName name="_nIncome">ModelApproach!$B$12</definedName>
+    <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
   <si>
     <t>Question</t>
   </si>
@@ -109,15 +113,28 @@
   <si>
     <t>E</t>
   </si>
+  <si>
+    <t>BrackLow</t>
+  </si>
+  <si>
+    <t>BrackHigh</t>
+  </si>
+  <si>
+    <t>Taxable</t>
+  </si>
+  <si>
+    <t>Error in rounding the tax</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +162,23 @@
       <family val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +203,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -399,10 +443,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -480,9 +526,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Intro_Hd" xfId="2" xr:uid="{E2C5C36D-925C-4CFF-BE88-5CFB3E213EB1}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{8373A6E1-9610-4091-8B0E-837676B7CF0A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1774,8 +1826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DC6B74-8320-4033-A242-06DF60A305BB}">
   <dimension ref="A1:O111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2533,4 +2585,875 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA8C9F0-E043-4ACC-B8BA-C492115F893E}">
+  <dimension ref="A1:O111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="3" width="11.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.296875" customWidth="1"/>
+    <col min="5" max="5" width="12.19921875" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="F1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="33"/>
+      <c r="H1" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="26">
+        <v>0</v>
+      </c>
+      <c r="C3" s="27">
+        <v>18200</v>
+      </c>
+      <c r="D3" s="28">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="24">
+        <v>60630</v>
+      </c>
+      <c r="H3" s="25">
+        <v>199920</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3"/>
+      <c r="O3"/>
+    </row>
+    <row r="4" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <f t="shared" ref="B4:B7" si="0">C3+1</f>
+        <v>18201</v>
+      </c>
+      <c r="C4" s="13">
+        <v>45000</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.19</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="16">
+        <v>1495</v>
+      </c>
+      <c r="H4" s="21">
+        <v>26068</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4"/>
+      <c r="O4"/>
+    </row>
+    <row r="5" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <f t="shared" si="0"/>
+        <v>45001</v>
+      </c>
+      <c r="C5" s="13">
+        <v>120000</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="16">
+        <v>25059</v>
+      </c>
+      <c r="H5" s="20">
+        <v>106439</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5"/>
+      <c r="O5"/>
+    </row>
+    <row r="6" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <f t="shared" si="0"/>
+        <v>120001</v>
+      </c>
+      <c r="C6" s="13">
+        <v>180000</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.37</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="16">
+        <v>1961</v>
+      </c>
+      <c r="H6" s="20">
+        <v>28521</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6"/>
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="14">
+        <f t="shared" si="0"/>
+        <v>180001</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="17">
+        <v>37816</v>
+      </c>
+      <c r="H7" s="22">
+        <v>142566</v>
+      </c>
+      <c r="K7"/>
+      <c r="O7"/>
+    </row>
+    <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="4"/>
+      <c r="D8"/>
+      <c r="E8" s="6"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="4"/>
+      <c r="D9"/>
+      <c r="E9" s="6"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="O9"/>
+    </row>
+    <row r="10" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="4"/>
+      <c r="D10"/>
+      <c r="E10" s="6"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+    </row>
+    <row r="11" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="4"/>
+      <c r="D11"/>
+      <c r="E11" s="6"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+    </row>
+    <row r="12" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="37">
+        <v>28521</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12"/>
+      <c r="E12" s="7"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="E13" s="7"/>
+      <c r="F13"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14" s="35">
+        <f>E20</f>
+        <v>1960.8</v>
+      </c>
+      <c r="J14" s="30" t="str" cm="1">
+        <f t="array" ref="J14:L19">_xlfn.VSTACK(F2:H2,_xlfn.HSTACK(F3:F7,H15:H19,H3:H7))</f>
+        <v>Person ID</v>
+      </c>
+      <c r="K14" s="30" t="str">
+        <v>Tax</v>
+      </c>
+      <c r="L14" s="31" t="str">
+        <v>Income</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="35" cm="1">
+        <f t="array" ref="B15:B19">B3:B7</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="35" cm="1">
+        <f t="array" ref="C15:C19">_xlfn.VSTACK(_xlfn.DROP(_xlfn.ANCHORARRAY(B15),1),B12)</f>
+        <v>18201</v>
+      </c>
+      <c r="D15" s="35">
+        <f>IF(_nIncome&lt;B15,0,MIN(C15,_nIncome)-B15)</f>
+        <v>18201</v>
+      </c>
+      <c r="E15" s="35" cm="1">
+        <f t="array" ref="E15:E19">D15:D19*D3:D7</f>
+        <v>0</v>
+      </c>
+      <c r="F15"/>
+      <c r="G15" s="38" cm="1">
+        <f t="array" ref="G15:G19">H3:H7</f>
+        <v>199920</v>
+      </c>
+      <c r="H15">
+        <f t="dataTable" ref="H15:H19" dt2D="0" dtr="0" r1="B12"/>
+        <v>60630.55</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="K15" s="24">
+        <v>60630.55</v>
+      </c>
+      <c r="L15" s="25">
+        <v>199920</v>
+      </c>
+      <c r="N15" t="b" cm="1">
+        <f t="array" ref="N15:O19">G3:H7=ROUND(K15:L19,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="35">
+        <v>18201</v>
+      </c>
+      <c r="C16" s="35">
+        <v>45001</v>
+      </c>
+      <c r="D16" s="35">
+        <f>IF(_nIncome&lt;B16,0,MIN(C16,_nIncome)-B16)</f>
+        <v>10320</v>
+      </c>
+      <c r="E16" s="35">
+        <v>1960.8</v>
+      </c>
+      <c r="F16"/>
+      <c r="G16">
+        <v>26068</v>
+      </c>
+      <c r="H16">
+        <v>1494.73</v>
+      </c>
+      <c r="J16" s="18" t="str">
+        <v>B</v>
+      </c>
+      <c r="K16" s="16">
+        <v>1494.73</v>
+      </c>
+      <c r="L16" s="21">
+        <v>26068</v>
+      </c>
+      <c r="N16" t="b">
+        <v>1</v>
+      </c>
+      <c r="O16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="35">
+        <v>45001</v>
+      </c>
+      <c r="C17" s="35">
+        <v>120001</v>
+      </c>
+      <c r="D17" s="35">
+        <f>IF(_nIncome&lt;B17,0,MIN(C17,_nIncome)-B17)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="35">
+        <v>0</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17">
+        <v>106439</v>
+      </c>
+      <c r="H17">
+        <v>25059.350000000002</v>
+      </c>
+      <c r="J17" s="18" t="str">
+        <v>C</v>
+      </c>
+      <c r="K17" s="16">
+        <v>25059.350000000002</v>
+      </c>
+      <c r="L17" s="20">
+        <v>106439</v>
+      </c>
+      <c r="N17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="35">
+        <v>120001</v>
+      </c>
+      <c r="C18" s="35">
+        <v>180001</v>
+      </c>
+      <c r="D18" s="35">
+        <f>IF(_nIncome&lt;B18,0,MIN(C18,_nIncome)-B18)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="35">
+        <v>0</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18">
+        <v>28521</v>
+      </c>
+      <c r="H18">
+        <v>1960.8</v>
+      </c>
+      <c r="J18" s="18" t="str">
+        <v>D</v>
+      </c>
+      <c r="K18" s="16">
+        <v>1960.8</v>
+      </c>
+      <c r="L18" s="20">
+        <v>28521</v>
+      </c>
+      <c r="N18" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="35">
+        <v>180001</v>
+      </c>
+      <c r="C19" s="35">
+        <v>28521</v>
+      </c>
+      <c r="D19" s="35">
+        <f>IF(_nIncome&lt;B19,0,MIN(C19,_nIncome)-B19)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="35">
+        <v>0</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19">
+        <v>142566</v>
+      </c>
+      <c r="H19">
+        <v>37816.050000000003</v>
+      </c>
+      <c r="J19" s="19" t="str">
+        <v>E</v>
+      </c>
+      <c r="K19" s="17">
+        <v>37816.050000000003</v>
+      </c>
+      <c r="L19" s="22">
+        <v>142566</v>
+      </c>
+      <c r="N19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="9"/>
+      <c r="E20" s="36">
+        <f>SUM(_xlfn.ANCHORARRAY(E15))</f>
+        <v>1960.8</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="9"/>
+      <c r="E21" s="1"/>
+      <c r="F21"/>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="9"/>
+      <c r="E22" s="1"/>
+      <c r="F22"/>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="9"/>
+      <c r="E23" s="1"/>
+      <c r="F23"/>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
+      <c r="E24" s="1"/>
+      <c r="F24"/>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+      <c r="E25" s="1"/>
+      <c r="F25"/>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="F26"/>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+      <c r="F27"/>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="9"/>
+      <c r="F28"/>
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="F29"/>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+      <c r="F30"/>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="F31"/>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
+      <c r="F32"/>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="F33"/>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="F34"/>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="F35"/>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="F36"/>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="F37"/>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="9"/>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="9"/>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="9"/>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="9"/>
+      <c r="F43" s="9"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="9"/>
+      <c r="F44" s="9"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="9"/>
+      <c r="F45" s="9"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="9"/>
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="9"/>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="9"/>
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="9"/>
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="9"/>
+      <c r="F52" s="9"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="9"/>
+      <c r="F53" s="9"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="9"/>
+      <c r="F54" s="9"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="9"/>
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="9"/>
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="9"/>
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="9"/>
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="9"/>
+      <c r="F59" s="9"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="9"/>
+      <c r="F60" s="9"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="9"/>
+      <c r="F61" s="9"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="9"/>
+      <c r="F62" s="9"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="9"/>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="9"/>
+      <c r="F64" s="9"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="9"/>
+      <c r="F65" s="9"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="9"/>
+      <c r="F66" s="9"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="9"/>
+      <c r="F67" s="9"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="9"/>
+      <c r="F68" s="9"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="9"/>
+      <c r="F69" s="9"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="9"/>
+      <c r="F70" s="9"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="9"/>
+      <c r="F71" s="9"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="9"/>
+      <c r="F72" s="9"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="9"/>
+      <c r="F73" s="9"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="9"/>
+      <c r="F74" s="9"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="9"/>
+      <c r="F75" s="9"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="9"/>
+      <c r="F76" s="9"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="9"/>
+      <c r="F77" s="9"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="9"/>
+      <c r="F78" s="9"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="9"/>
+      <c r="F79" s="9"/>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="9"/>
+      <c r="F80" s="9"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="9"/>
+      <c r="F81" s="9"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="9"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F83" s="9"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="9"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="9"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="9"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F87" s="9"/>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F88" s="9"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="9"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="9"/>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="9"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="9"/>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F93" s="9"/>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="9"/>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F95" s="9"/>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F96" s="9"/>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="9"/>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="9"/>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="9"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="9"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F101" s="9"/>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F102" s="9"/>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F103" s="9"/>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F104" s="9"/>
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F105" s="9"/>
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F106" s="9"/>
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F107" s="9"/>
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F108" s="9"/>
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F109" s="9"/>
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F110" s="9"/>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F111" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Minor cleanup. I am done here.
</commit_message>
<xml_diff>
--- a/CH-076 Reverse Stepped Tax.xlsx
+++ b/CH-076 Reverse Stepped Tax.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892CB068-4B71-4060-A1F2-B1362BA1A7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AC7D5F-463B-48F4-B78B-1243DF27D2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2592,7 +2592,7 @@
   <dimension ref="A1:O111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>